<commit_message>
Se Finaliza Vista de detalle de compras
</commit_message>
<xml_diff>
--- a/Documentacion/Cronograma Sifweb.xlsx
+++ b/Documentacion/Cronograma Sifweb.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Tarea</t>
   </si>
@@ -135,12 +135,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -185,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -193,10 +199,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,19 +518,19 @@
     <col min="2" max="3" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
@@ -563,17 +571,17 @@
       </c>
     </row>
     <row r="7" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="3" t="s">
+      <c r="F7" s="10"/>
+      <c r="G7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="9">
         <v>80</v>
       </c>
     </row>
@@ -627,10 +635,10 @@
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H11" s="3">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -641,8 +649,12 @@
         <v>11</v>
       </c>
       <c r="F12" s="5"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="3">
+        <v>100</v>
+      </c>
     </row>
     <row r="13" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="3" t="s">
@@ -693,15 +705,15 @@
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D18" s="6" t="s">
@@ -737,10 +749,10 @@
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="7" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>